<commit_message>
Added Array files, updates to excel, data provider, listener, base class and Tests
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10296" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>username</t>
   </si>
@@ -78,78 +78,63 @@
     <t>PracticeQuestion</t>
   </si>
   <si>
-    <t>Run Output</t>
-  </si>
-  <si>
-    <t>Submit output</t>
-  </si>
-  <si>
-    <t>def search(input_list, num):
-  if(num in input_list):
-    print("Element Found")
-  else:
-    print("Not Found")
-search([12, 23, 45, 67, 6, 90] , 12)</t>
-  </si>
-  <si>
-    <t>def findMaxConsecutiveOnes(nums):
-    max_count = 0
-    current_count = 0
-    for num in nums:
-        if num == 1:
-            current_count += 1
-            max_count = max(max_count, current_count)
-        else:
-            current_count = 0
-    return max_count
-nums = [1, 1, 0, 1, 1, 1]
-print(findMaxConsecutiveOnes(nums))</t>
-  </si>
-  <si>
-    <t>def findNumbers(nums):
-    count = 0
-    for num in nums:
-        if len(str(num)) % 2 == 0:
-            count += 1
-    return count
-nums = [54521, 25, 46, 17896]
-print(findNumbers(nums))</t>
-  </si>
-  <si>
-    <t>def sortedSquares(nums):
-    result = []
-    left, right = 0, len(nums) - 1
-    while left &lt;= right:
-        if abs(nums[left]) &gt; abs(nums[right]):
-            result.append(nums[left] ** 2)
-            left += 1
-        else:
-            result.append(nums[right] ** 2)
-            right -= 1
-    return result[::-1]
-nums = [-4, -1, 0, 3, 10]
-print(sortedSquares(nums))</t>
-  </si>
-  <si>
-    <t>def findMaxConsecutiveOnes(nums):~
-max_count = 0
-@current_count = 0
-for num in nums:
-if num == 1:
-current_count += 1
-max_count = max(max_count, current_count)
-else:
-current_count = 0
-return max_count
-nums = [1, 1, 0, 1, 1, 1]
-print(findMaxConsecutiveOnes(nums))</t>
+    <t>Drop-down</t>
+  </si>
+  <si>
+    <t>Data Structures</t>
+  </si>
+  <si>
+    <t>Arrays</t>
+  </si>
+  <si>
+    <t>Linked List</t>
+  </si>
+  <si>
+    <t>Stack</t>
+  </si>
+  <si>
+    <t>Queue</t>
+  </si>
+  <si>
+    <t>Tree</t>
+  </si>
+  <si>
+    <t>Graph</t>
+  </si>
+  <si>
+    <t>@def search(input_list, num):~if(num in input_list): ~print("Element Found")~@@else:~print("Not Found")~@@@@search([12, 23, 45, 67, 6, 90] , 12)</t>
+  </si>
+  <si>
+    <t>@def findMaxConsecutiveOnes(nums):~max_count = 0~current_count = 0~for num in nums:~  if num == 1:~         @@@@@@@current_count += 1~max_count = max(max_count, current_count)~@@@@else:~   @current_count = 0~@@@@@@@@return max_count~nums = [1, 1, 0, 1, 1, 1]~print(findMaxConsecutiveOnes(nums))</t>
+  </si>
+  <si>
+    <t>@def findNumbers(nums):~  count = 0~  @@for num in nums:~  if len(str(num)) % 2 == 0:~         @@@@@@@count += 1~@@@@@@@@return count~@@nums = [54521, 25, 46, 17896]~ @print(findNumbers(nums))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@def sortedSquares(nums):~  result = []~  @@left, right = 0, len(nums) - 1~  @@while left &lt;= right:~  if abs(nums[left]) &gt; abs(nums[right]):~         @@@@@@@result.append(nums[left] ** 2)~         @@@@@@@@@left += 1~   @@@@@@@else:~   @result.append(nums[right] ** 2)~   @@@right -= 1~  @@@@@@@@@@return result[::-1]~@@nums = [-4, -1, 0, 3, 10]~ @print(sortedSquares(nums))
+</t>
+  </si>
+  <si>
+    <t>Second last try</t>
+  </si>
+  <si>
+    <t>OutputElement Found</t>
+  </si>
+  <si>
+    <t>Output3</t>
+  </si>
+  <si>
+    <t>Output2</t>
+  </si>
+  <si>
+    <t>Output[0, 1, 9, 16, 100]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +167,11 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -236,14 +226,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -549,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -639,17 +629,63 @@
         <v>7</v>
       </c>
     </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B2" r:id="rId3"/>
-    <hyperlink ref="A7" r:id="rId4" display="Jewel@"/>
-    <hyperlink ref="B7" r:id="rId5"/>
-    <hyperlink ref="B6" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B10" r:id="rId8"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -699,56 +735,62 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="106.6640625" customWidth="1"/>
+    <col min="1" max="1" width="207.33203125" customWidth="1"/>
     <col min="2" max="2" width="14.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="86.4">
-      <c r="A2" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="172.8">
-      <c r="A3" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="115.2">
-      <c r="A4" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="187.2">
-      <c r="A5" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="172.8">
-      <c r="A6" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="5"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="28.8">
+      <c r="A3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="43.2">
+      <c r="A5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>